<commit_message>
Modificaciones a la clase PageInstituciones
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A317B86-3789-46C8-8E32-13067CD62D3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18011D5E-AE9E-4332-A6EB-363EF3CA4B23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="46">
   <si>
     <t>18092588-0</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>DEC_0089</t>
+  </si>
+  <si>
+    <t>DEC_0101</t>
+  </si>
+  <si>
+    <t>DEC_0102</t>
   </si>
 </sst>
 </file>
@@ -496,7 +502,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1123,12 +1129,32 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="A20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="A21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>

</xml_diff>

<commit_message>
Se agregan los scripts 0101/0104/0105/0106/0107/0108/0109 en la clase Tests_AdmInstituciones
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91574864-D3C5-449F-B183-4670FE858B26}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD45F6D7-022D-46E4-BE8C-AEA38DF05C38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="70">
   <si>
     <t>18092588-0</t>
   </si>
@@ -172,6 +172,78 @@
   </si>
   <si>
     <t>DEC_0104</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 104</t>
+  </si>
+  <si>
+    <t>DEC_0105</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 105</t>
+  </si>
+  <si>
+    <t>DEC_0106</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 106</t>
+  </si>
+  <si>
+    <t>DEC_0107</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 107</t>
+  </si>
+  <si>
+    <t>DEC_0108</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 108</t>
+  </si>
+  <si>
+    <t>DEC_0109</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 109</t>
+  </si>
+  <si>
+    <t>DEC_0110</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 110</t>
+  </si>
+  <si>
+    <t>DEC_0111</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 111</t>
+  </si>
+  <si>
+    <t>DEC_0112</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 112</t>
+  </si>
+  <si>
+    <t>DEC_0113</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 113</t>
+  </si>
+  <si>
+    <t>DEC_0114</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 114</t>
+  </si>
+  <si>
+    <t>DEC_0115</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 115</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 101</t>
   </si>
 </sst>
 </file>
@@ -499,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1141,6 +1213,24 @@
       <c r="D20" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="E20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
@@ -1155,68 +1245,494 @@
       <c r="D21" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="E21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="A22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
+      <c r="A23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
+      <c r="A24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
+      <c r="A25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
+      <c r="A26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
+      <c r="A27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
+      <c r="A28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
+      <c r="A29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
+      <c r="A30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="A31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B34" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B35" s="2" t="s">
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B54" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B55" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1239,8 +1755,34 @@
     <hyperlink ref="J18" r:id="rId14" display="pruebaAutomationQA@acepta.com" xr:uid="{4AF23467-E418-4F78-AC16-2ABA00FFFD0C}"/>
     <hyperlink ref="J19" r:id="rId15" xr:uid="{DBC43BFD-1FCA-49DD-BE7A-65A4110EB1DB}"/>
     <hyperlink ref="H19" r:id="rId16" xr:uid="{800C91D9-90CE-4DAC-B7B1-7F455580E2BE}"/>
+    <hyperlink ref="J21" r:id="rId17" xr:uid="{1C7833E9-13B5-4AF2-AEA5-D63026801CAA}"/>
+    <hyperlink ref="H21" r:id="rId18" xr:uid="{4C7F7FBE-6633-4F1A-AF4B-6CB76ADA45CD}"/>
+    <hyperlink ref="J22" r:id="rId19" xr:uid="{846BC360-9D01-4EE9-BC3E-8058894A1E5C}"/>
+    <hyperlink ref="J23" r:id="rId20" xr:uid="{F01CD034-6450-4B27-BF7F-DCB223C7D84E}"/>
+    <hyperlink ref="J24" r:id="rId21" xr:uid="{EB9B0CD8-B7E8-4CE7-AC1D-8575D41FD985}"/>
+    <hyperlink ref="J25" r:id="rId22" xr:uid="{1A519B6D-0F7F-4EF9-A08F-130B06CB42F1}"/>
+    <hyperlink ref="J26" r:id="rId23" xr:uid="{8637C55C-7876-425E-99D7-A3FA49DC8A31}"/>
+    <hyperlink ref="H22" r:id="rId24" xr:uid="{630BCDEA-092F-4569-828A-3F7D0110243D}"/>
+    <hyperlink ref="H23" r:id="rId25" xr:uid="{E371DA47-9293-444F-A347-449EDAF19D47}"/>
+    <hyperlink ref="H24" r:id="rId26" xr:uid="{78F4FEB1-14BA-451A-9944-497220B745BB}"/>
+    <hyperlink ref="H25" r:id="rId27" xr:uid="{9D9294DA-BBE2-4874-8AF5-8A2315C2A662}"/>
+    <hyperlink ref="H26" r:id="rId28" xr:uid="{52B65006-F086-4CC4-9300-A169B36E3A6E}"/>
+    <hyperlink ref="J27" r:id="rId29" xr:uid="{4DEE69B5-C2AD-454B-987C-5E0B848D41D9}"/>
+    <hyperlink ref="H27" r:id="rId30" xr:uid="{7A9FFDCE-E1FC-410B-A918-AED72AF15E96}"/>
+    <hyperlink ref="J28" r:id="rId31" xr:uid="{B8B5754F-30A1-4268-8AC4-43D9E8DA843D}"/>
+    <hyperlink ref="J29" r:id="rId32" xr:uid="{C948DE30-BD08-45FD-B093-CDC915B0B7E5}"/>
+    <hyperlink ref="J30" r:id="rId33" xr:uid="{6D6872DA-F694-4DBF-B4D6-FA6B451AD7D0}"/>
+    <hyperlink ref="J31" r:id="rId34" xr:uid="{56F9ADA4-838D-4A73-B944-AFC620E95E64}"/>
+    <hyperlink ref="H28" r:id="rId35" xr:uid="{135DA600-F746-40E5-AC5E-2AF15ED408A4}"/>
+    <hyperlink ref="H29" r:id="rId36" xr:uid="{D347EA6E-C39D-4211-A51F-FC4C68952D37}"/>
+    <hyperlink ref="H30" r:id="rId37" xr:uid="{DC7A020C-9525-4F8F-917D-77E829339688}"/>
+    <hyperlink ref="H31" r:id="rId38" xr:uid="{1DE13343-8DDE-490F-8924-884D2E9F4F92}"/>
+    <hyperlink ref="J32" r:id="rId39" xr:uid="{FF88120D-113C-4997-931C-6E4EA388397B}"/>
+    <hyperlink ref="H32" r:id="rId40" xr:uid="{1D6EBFC5-C948-4616-99C9-AEF53717B7A9}"/>
+    <hyperlink ref="J20" r:id="rId41" xr:uid="{6AF1CB49-DA1E-4717-B2CB-A21CF8C0E5B2}"/>
+    <hyperlink ref="H20" r:id="rId42" xr:uid="{AD819D11-0D28-49B1-97A0-FA4E8EFA82B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agregan los scripts 0116/0116/0117/0118/0119/0120 a la clase Tests_AdmInstituciones
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD45F6D7-022D-46E4-BE8C-AEA38DF05C38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA8B572-82C3-401A-A5A3-6AACF680E7D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="90">
   <si>
     <t>18092588-0</t>
   </si>
@@ -244,6 +244,66 @@
   </si>
   <si>
     <t>Nueva Empresa QA 101</t>
+  </si>
+  <si>
+    <t>DEC_0116</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 116</t>
+  </si>
+  <si>
+    <t>DEC_0117</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 117</t>
+  </si>
+  <si>
+    <t>DEC_0118</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 118</t>
+  </si>
+  <si>
+    <t>DEC_0119</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 119</t>
+  </si>
+  <si>
+    <t>DEC_0120</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 120</t>
+  </si>
+  <si>
+    <t>DEC_0121</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 121</t>
+  </si>
+  <si>
+    <t>DEC_0122</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 122</t>
+  </si>
+  <si>
+    <t>DEC_0123</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 123</t>
+  </si>
+  <si>
+    <t>DEC_0124</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 124</t>
+  </si>
+  <si>
+    <t>DEC_0125</t>
+  </si>
+  <si>
+    <t>Nueva Empresa QA 125</t>
   </si>
 </sst>
 </file>
@@ -574,7 +634,7 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:B32"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1616,82 +1676,352 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="H40" s="4"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="H41" s="4"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="H42" s="4"/>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="H43" s="4"/>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="H44" s="4"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="H45" s="4"/>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="H46" s="4"/>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="H47" s="4"/>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="H48" s="4"/>
@@ -1781,8 +2111,28 @@
     <hyperlink ref="H32" r:id="rId40" xr:uid="{1D6EBFC5-C948-4616-99C9-AEF53717B7A9}"/>
     <hyperlink ref="J20" r:id="rId41" xr:uid="{6AF1CB49-DA1E-4717-B2CB-A21CF8C0E5B2}"/>
     <hyperlink ref="H20" r:id="rId42" xr:uid="{AD819D11-0D28-49B1-97A0-FA4E8EFA82B0}"/>
+    <hyperlink ref="J33" r:id="rId43" xr:uid="{CC8E2CC9-875E-4CC6-A539-DB5AA1D43FE5}"/>
+    <hyperlink ref="J34" r:id="rId44" xr:uid="{64175105-E97E-48B8-ABF2-3786D7BB6F58}"/>
+    <hyperlink ref="J35" r:id="rId45" xr:uid="{FDBBD802-18E9-46D2-9452-534EFA3BFD42}"/>
+    <hyperlink ref="J36" r:id="rId46" xr:uid="{55345BC2-C233-40BD-9349-E7A0957270CB}"/>
+    <hyperlink ref="J37" r:id="rId47" xr:uid="{EC0BB78F-765A-42B1-8037-AF4E8558857A}"/>
+    <hyperlink ref="J38" r:id="rId48" xr:uid="{A74BF8C4-70BC-4BEF-95ED-58DC0372901C}"/>
+    <hyperlink ref="J39" r:id="rId49" xr:uid="{10AA3DC8-AC70-4375-BCCD-F18592D5B0DF}"/>
+    <hyperlink ref="J40" r:id="rId50" xr:uid="{7824B783-083A-4457-87B2-52B7850329B1}"/>
+    <hyperlink ref="J41" r:id="rId51" xr:uid="{FA1FA667-BBA3-4CA9-B506-0C1A80F6097C}"/>
+    <hyperlink ref="J42" r:id="rId52" xr:uid="{D8F26B92-64E4-4A0B-87C3-56E7E21F14B1}"/>
+    <hyperlink ref="H33" r:id="rId53" xr:uid="{F4020C80-1696-4779-8A55-E73FE0942D0F}"/>
+    <hyperlink ref="H34" r:id="rId54" xr:uid="{CCF95056-1573-48BD-A8DB-947E4D63F41F}"/>
+    <hyperlink ref="H35" r:id="rId55" xr:uid="{6BC30BF1-12A9-4C4C-9AE3-8CE8E4186337}"/>
+    <hyperlink ref="H36" r:id="rId56" xr:uid="{D6166970-AEC1-4B06-B3C8-EC072F439498}"/>
+    <hyperlink ref="H37" r:id="rId57" xr:uid="{A56B8264-F0A2-46B8-AF33-A77D04029E3D}"/>
+    <hyperlink ref="H38" r:id="rId58" xr:uid="{F2072910-61C2-40CF-B6A9-A2D91E3E7E25}"/>
+    <hyperlink ref="H39" r:id="rId59" xr:uid="{99AC6171-FD63-4750-A3D4-D6B83CD0FA22}"/>
+    <hyperlink ref="H40" r:id="rId60" xr:uid="{9D839C08-016D-40CE-BA98-A475D9A65C0B}"/>
+    <hyperlink ref="H41" r:id="rId61" xr:uid="{BB9C329A-ABE1-4A3C-89C7-3A9343F7F556}"/>
+    <hyperlink ref="H42" r:id="rId62" xr:uid="{38A6C37D-7666-4A63-94F0-81E6B10288CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId43"/>
+  <pageSetup orientation="portrait" r:id="rId63"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega Metodo EditarInstitucion en clase PageInstituciones // Se agrega script 0124 a la clase Tests_AdmInstituciones
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA8B572-82C3-401A-A5A3-6AACF680E7D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB608296-6883-497D-9879-3E5E22873889}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="94">
   <si>
     <t>18092588-0</t>
   </si>
@@ -297,13 +297,25 @@
     <t>DEC_0124</t>
   </si>
   <si>
-    <t>Nueva Empresa QA 124</t>
-  </si>
-  <si>
     <t>DEC_0125</t>
   </si>
   <si>
-    <t>Nueva Empresa QA 125</t>
+    <t>DEC_0126</t>
+  </si>
+  <si>
+    <t>DEC_0127</t>
+  </si>
+  <si>
+    <t>DEC_0128</t>
+  </si>
+  <si>
+    <t>DEC_0129</t>
+  </si>
+  <si>
+    <t>DEC_0130</t>
+  </si>
+  <si>
+    <t>DEC_0131</t>
   </si>
 </sst>
 </file>
@@ -631,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1942,88 +1954,90 @@
       <c r="C41" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="H41" s="4"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E42" s="1" t="s">
+      <c r="B43" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="H43" s="4"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
+      <c r="B44" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="H44" s="4"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
+      <c r="A45" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="H45" s="4"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
+      <c r="A46" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="H46" s="4"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
+      <c r="A47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="H47" s="4"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
+      <c r="A48" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="H48" s="4"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.3">
@@ -2044,25 +2058,20 @@
     <row r="52" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
-      <c r="H52" s="4"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
+      <c r="B53" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B54" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B55" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C54" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2119,20 +2128,16 @@
     <hyperlink ref="J38" r:id="rId48" xr:uid="{A74BF8C4-70BC-4BEF-95ED-58DC0372901C}"/>
     <hyperlink ref="J39" r:id="rId49" xr:uid="{10AA3DC8-AC70-4375-BCCD-F18592D5B0DF}"/>
     <hyperlink ref="J40" r:id="rId50" xr:uid="{7824B783-083A-4457-87B2-52B7850329B1}"/>
-    <hyperlink ref="J41" r:id="rId51" xr:uid="{FA1FA667-BBA3-4CA9-B506-0C1A80F6097C}"/>
-    <hyperlink ref="J42" r:id="rId52" xr:uid="{D8F26B92-64E4-4A0B-87C3-56E7E21F14B1}"/>
-    <hyperlink ref="H33" r:id="rId53" xr:uid="{F4020C80-1696-4779-8A55-E73FE0942D0F}"/>
-    <hyperlink ref="H34" r:id="rId54" xr:uid="{CCF95056-1573-48BD-A8DB-947E4D63F41F}"/>
-    <hyperlink ref="H35" r:id="rId55" xr:uid="{6BC30BF1-12A9-4C4C-9AE3-8CE8E4186337}"/>
-    <hyperlink ref="H36" r:id="rId56" xr:uid="{D6166970-AEC1-4B06-B3C8-EC072F439498}"/>
-    <hyperlink ref="H37" r:id="rId57" xr:uid="{A56B8264-F0A2-46B8-AF33-A77D04029E3D}"/>
-    <hyperlink ref="H38" r:id="rId58" xr:uid="{F2072910-61C2-40CF-B6A9-A2D91E3E7E25}"/>
-    <hyperlink ref="H39" r:id="rId59" xr:uid="{99AC6171-FD63-4750-A3D4-D6B83CD0FA22}"/>
-    <hyperlink ref="H40" r:id="rId60" xr:uid="{9D839C08-016D-40CE-BA98-A475D9A65C0B}"/>
-    <hyperlink ref="H41" r:id="rId61" xr:uid="{BB9C329A-ABE1-4A3C-89C7-3A9343F7F556}"/>
-    <hyperlink ref="H42" r:id="rId62" xr:uid="{38A6C37D-7666-4A63-94F0-81E6B10288CD}"/>
+    <hyperlink ref="H33" r:id="rId51" xr:uid="{F4020C80-1696-4779-8A55-E73FE0942D0F}"/>
+    <hyperlink ref="H34" r:id="rId52" xr:uid="{CCF95056-1573-48BD-A8DB-947E4D63F41F}"/>
+    <hyperlink ref="H35" r:id="rId53" xr:uid="{6BC30BF1-12A9-4C4C-9AE3-8CE8E4186337}"/>
+    <hyperlink ref="H36" r:id="rId54" xr:uid="{D6166970-AEC1-4B06-B3C8-EC072F439498}"/>
+    <hyperlink ref="H37" r:id="rId55" xr:uid="{A56B8264-F0A2-46B8-AF33-A77D04029E3D}"/>
+    <hyperlink ref="H38" r:id="rId56" xr:uid="{F2072910-61C2-40CF-B6A9-A2D91E3E7E25}"/>
+    <hyperlink ref="H39" r:id="rId57" xr:uid="{99AC6171-FD63-4750-A3D4-D6B83CD0FA22}"/>
+    <hyperlink ref="H40" r:id="rId58" xr:uid="{9D839C08-016D-40CE-BA98-A475D9A65C0B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId63"/>
+  <pageSetup orientation="portrait" r:id="rId59"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agregan los script 0125/0126/0127/0128/129/130 a la Clase Tests_AdmInstituciones
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB608296-6883-497D-9879-3E5E22873889}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2269D747-DC34-4556-A62E-A3C5A239069B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="95">
   <si>
     <t>18092588-0</t>
   </si>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>DEC_0131</t>
+  </si>
+  <si>
+    <t>Verity1.1</t>
   </si>
 </sst>
 </file>
@@ -645,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -928,7 +931,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>17</v>
@@ -960,7 +963,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>17</v>
@@ -992,7 +995,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>17</v>
@@ -1024,7 +1027,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>17</v>
@@ -1056,7 +1059,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>17</v>
@@ -1088,7 +1091,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>17</v>
@@ -1120,7 +1123,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
@@ -1152,7 +1155,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>17</v>
@@ -1184,7 +1187,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>17</v>
@@ -1216,7 +1219,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>17</v>
@@ -1248,7 +1251,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>17</v>
@@ -1280,7 +1283,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>17</v>
@@ -1312,7 +1315,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>17</v>
@@ -1344,7 +1347,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>17</v>
@@ -1376,7 +1379,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>17</v>
@@ -1408,7 +1411,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>17</v>
@@ -1440,7 +1443,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>17</v>
@@ -1472,7 +1475,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>17</v>
@@ -1504,7 +1507,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>17</v>
@@ -1536,7 +1539,7 @@
         <v>2</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>17</v>
@@ -1568,7 +1571,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>17</v>
@@ -1600,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>17</v>
@@ -1632,7 +1635,7 @@
         <v>2</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>17</v>
@@ -1664,7 +1667,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>17</v>
@@ -1696,7 +1699,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>17</v>
@@ -1728,7 +1731,7 @@
         <v>2</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>17</v>
@@ -1760,7 +1763,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>17</v>
@@ -1792,7 +1795,7 @@
         <v>2</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>17</v>
@@ -1824,7 +1827,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>17</v>
@@ -1856,7 +1859,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>17</v>
@@ -1888,7 +1891,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>17</v>
@@ -1920,7 +1923,7 @@
         <v>2</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>17</v>
@@ -1952,9 +1955,29 @@
         <v>2</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H41" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
@@ -1964,9 +1987,29 @@
         <v>2</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H42" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
@@ -1976,9 +2019,29 @@
         <v>2</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H43" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
@@ -1988,9 +2051,29 @@
         <v>2</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H44" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
@@ -2000,9 +2083,29 @@
         <v>2</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H45" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
@@ -2012,9 +2115,29 @@
         <v>2</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H46" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
@@ -2024,9 +2147,29 @@
         <v>2</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H47" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
@@ -2036,9 +2179,29 @@
         <v>2</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H48" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B49" s="4"/>

</xml_diff>

<commit_message>
Se agregan los script 0131/0132/0133/0134/0135 a la Clase Tests_AdmInstituciones
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2269D747-DC34-4556-A62E-A3C5A239069B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F0FF56-3DC4-4428-9B32-E40A0EB5CE1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="110">
   <si>
     <t>18092588-0</t>
   </si>
@@ -319,6 +319,51 @@
   </si>
   <si>
     <t>Verity1.1</t>
+  </si>
+  <si>
+    <t>DEC_0132</t>
+  </si>
+  <si>
+    <t>DEC_0133</t>
+  </si>
+  <si>
+    <t>DEC_0134</t>
+  </si>
+  <si>
+    <t>DEC_0135</t>
+  </si>
+  <si>
+    <t>DEC_0136</t>
+  </si>
+  <si>
+    <t>DEC_0137</t>
+  </si>
+  <si>
+    <t>DEC_0138</t>
+  </si>
+  <si>
+    <t>DEC_0139</t>
+  </si>
+  <si>
+    <t>DEC_0140</t>
+  </si>
+  <si>
+    <t>DEC_0141</t>
+  </si>
+  <si>
+    <t>DEC_0142</t>
+  </si>
+  <si>
+    <t>DEC_0143</t>
+  </si>
+  <si>
+    <t>DEC_0144</t>
+  </si>
+  <si>
+    <t>DEC_0145</t>
+  </si>
+  <si>
+    <t>DEC_0146</t>
   </si>
 </sst>
 </file>
@@ -646,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2203,38 +2248,503 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="H49" s="4"/>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="H50" s="4"/>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="H51" s="4"/>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="B53" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C53" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B65" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B54" s="2" t="s">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B66" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agregan los scripts 0146/0147/0148/0149 a la clase Tests_AdmInstituciones
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A298415-0817-4E12-A267-9455EB95C27C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF9C0B7-1E7A-4E1F-945C-5E0AF730D627}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="119">
   <si>
     <t>18092588-0</t>
   </si>
@@ -364,6 +364,33 @@
   </si>
   <si>
     <t>DEC_0146</t>
+  </si>
+  <si>
+    <t>DEC_0147</t>
+  </si>
+  <si>
+    <t>DEC_0148</t>
+  </si>
+  <si>
+    <t>DEC_0149</t>
+  </si>
+  <si>
+    <t>DEC_0150</t>
+  </si>
+  <si>
+    <t>DEC_0151</t>
+  </si>
+  <si>
+    <t>DEC_0152</t>
+  </si>
+  <si>
+    <t>DEC_0153</t>
+  </si>
+  <si>
+    <t>DEC_0154</t>
+  </si>
+  <si>
+    <t>DEC_0155</t>
   </si>
 </sst>
 </file>
@@ -691,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2729,22 +2756,318 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="B65" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C65" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B76" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C76" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B66" s="2" t="s">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B77" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C77" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualizando proyecto antes de comenzar agregar scripts
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF9C0B7-1E7A-4E1F-945C-5E0AF730D627}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CC9274-3CA1-45D7-ABEA-5BD18E1007B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="127">
   <si>
     <t>18092588-0</t>
   </si>
@@ -391,6 +391,30 @@
   </si>
   <si>
     <t>DEC_0155</t>
+  </si>
+  <si>
+    <t>DEC_0156</t>
+  </si>
+  <si>
+    <t>DEC_0157</t>
+  </si>
+  <si>
+    <t>DEC_0158</t>
+  </si>
+  <si>
+    <t>DEC_0159</t>
+  </si>
+  <si>
+    <t>DEC_0160</t>
+  </si>
+  <si>
+    <t>DEC_0161</t>
+  </si>
+  <si>
+    <t>DEC_0162</t>
+  </si>
+  <si>
+    <t>DEC_0163</t>
   </si>
 </sst>
 </file>
@@ -718,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3044,30 +3068,290 @@
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B73" s="4"/>
-      <c r="C73" s="4"/>
+      <c r="A73" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
+      <c r="A74" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
+      <c r="A75" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="B76" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C76" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J80" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B85" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C85" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B77" s="2" t="s">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B86" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="C86" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agrega script 0159 a la clase Tests_AdmInstituciones
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CC9274-3CA1-45D7-ABEA-5BD18E1007B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9965CC-4B9D-49B7-B3F3-8CBFB2596EF8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -745,7 +745,7 @@
   <dimension ref="A1:J86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Se agregan los scripts 0161/0163 a la clase Tests_AdmInstituciones. Tambíén se crea la clase PageAplicaciones para los componentes de la opción Aplicaciones
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9965CC-4B9D-49B7-B3F3-8CBFB2596EF8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6A5066-EAD7-4459-A200-20E29C7725F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="139">
   <si>
     <t>18092588-0</t>
   </si>
@@ -415,6 +415,42 @@
   </si>
   <si>
     <t>DEC_0163</t>
+  </si>
+  <si>
+    <t>DEC_0164</t>
+  </si>
+  <si>
+    <t>DEC_0165</t>
+  </si>
+  <si>
+    <t>DEC_0166</t>
+  </si>
+  <si>
+    <t>DEC_0167</t>
+  </si>
+  <si>
+    <t>DEC_0168</t>
+  </si>
+  <si>
+    <t>DEC_0169</t>
+  </si>
+  <si>
+    <t>DEC_0170</t>
+  </si>
+  <si>
+    <t>DEC_0171</t>
+  </si>
+  <si>
+    <t>DEC_0172</t>
+  </si>
+  <si>
+    <t>DEC_0173</t>
+  </si>
+  <si>
+    <t>DEC_0174</t>
+  </si>
+  <si>
+    <t>DEC_0175</t>
   </si>
 </sst>
 </file>
@@ -742,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J86"/>
+  <dimension ref="A1:J96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3323,35 +3359,411 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B82" s="4"/>
-      <c r="C82" s="4"/>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B83" s="4"/>
-      <c r="C83" s="4"/>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J84" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="B85" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C85" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J86" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J87" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J89" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I90" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J90" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J91" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J92" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B95" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B86" s="2" t="s">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B96" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="C96" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agregan los scripts 0165/0166 a la clase Tests_AdmInstituciones
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6A5066-EAD7-4459-A200-20E29C7725F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCC4713-9649-440E-8F21-BE079645DE1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="154">
   <si>
     <t>18092588-0</t>
   </si>
@@ -451,6 +451,51 @@
   </si>
   <si>
     <t>DEC_0175</t>
+  </si>
+  <si>
+    <t>DEC_0176</t>
+  </si>
+  <si>
+    <t>DEC_0177</t>
+  </si>
+  <si>
+    <t>DEC_0178</t>
+  </si>
+  <si>
+    <t>DEC_0179</t>
+  </si>
+  <si>
+    <t>DEC_0180</t>
+  </si>
+  <si>
+    <t>DEC_0181</t>
+  </si>
+  <si>
+    <t>DEC_0182</t>
+  </si>
+  <si>
+    <t>DEC_0183</t>
+  </si>
+  <si>
+    <t>DEC_0184</t>
+  </si>
+  <si>
+    <t>DEC_0185</t>
+  </si>
+  <si>
+    <t>DEC_0186</t>
+  </si>
+  <si>
+    <t>DEC_0187</t>
+  </si>
+  <si>
+    <t>DEC_0188</t>
+  </si>
+  <si>
+    <t>DEC_0189</t>
+  </si>
+  <si>
+    <t>DEC_0190</t>
   </si>
 </sst>
 </file>
@@ -778,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J96"/>
+  <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="H101" sqref="H101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3744,26 +3789,502 @@
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B93" s="4"/>
-      <c r="C93" s="4"/>
+      <c r="A93" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B94" s="4"/>
-      <c r="C94" s="4"/>
+      <c r="A94" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="B95" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C95" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J102" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I103" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J103" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J105" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I106" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J106" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B109" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C109" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B96" s="2" t="s">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B110" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="C110" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agregan los scripts 0187/0196/0197 a la clase Tests_AdmInstituciones
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCC4713-9649-440E-8F21-BE079645DE1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1450EA7A-4DC3-47E1-88C6-0089B4A68445}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="164">
   <si>
     <t>18092588-0</t>
   </si>
@@ -496,6 +496,36 @@
   </si>
   <si>
     <t>DEC_0190</t>
+  </si>
+  <si>
+    <t>DEC_0191</t>
+  </si>
+  <si>
+    <t>DEC_0192</t>
+  </si>
+  <si>
+    <t>DEC_0193</t>
+  </si>
+  <si>
+    <t>DEC_0194</t>
+  </si>
+  <si>
+    <t>DEC_0195</t>
+  </si>
+  <si>
+    <t>DEC_0196</t>
+  </si>
+  <si>
+    <t>DEC_0197</t>
+  </si>
+  <si>
+    <t>DEC_0198</t>
+  </si>
+  <si>
+    <t>DEC_0199</t>
+  </si>
+  <si>
+    <t>DEC_0200</t>
   </si>
 </sst>
 </file>
@@ -823,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J110"/>
+  <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="H101" sqref="H101"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104:C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4144,11 +4174,11 @@
       <c r="A104" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B104" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C104" s="4" t="s">
-        <v>94</v>
+      <c r="B104" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>16</v>
@@ -4176,11 +4206,11 @@
       <c r="A105" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B105" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>94</v>
+      <c r="B105" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>16</v>
@@ -4208,11 +4238,11 @@
       <c r="A106" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B106" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C106" s="4" t="s">
-        <v>94</v>
+      <c r="B106" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>16</v>
@@ -4240,11 +4270,11 @@
       <c r="A107" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B107" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>94</v>
+      <c r="B107" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>16</v>
@@ -4269,22 +4299,342 @@
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B108" s="4"/>
-      <c r="C108" s="4"/>
+      <c r="A108" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B109" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C109" s="4" t="s">
-        <v>3</v>
+      <c r="A109" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>156</v>
+      </c>
       <c r="B110" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C110" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J111" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I112" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J112" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J113" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J114" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I115" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J115" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I116" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J116" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I117" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J117" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B118" s="4"/>
+      <c r="C118" s="4"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B119" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B120" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C120" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se crea la clase Tests_Usuarios con los scripts respectivos
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1450EA7A-4DC3-47E1-88C6-0089B4A68445}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A35A1F-52F4-413D-A106-F63E76134443}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="184">
   <si>
     <t>18092588-0</t>
   </si>
@@ -526,6 +526,66 @@
   </si>
   <si>
     <t>DEC_0200</t>
+  </si>
+  <si>
+    <t>DEC_0201</t>
+  </si>
+  <si>
+    <t>DEC_0202</t>
+  </si>
+  <si>
+    <t>DEC_0203</t>
+  </si>
+  <si>
+    <t>DEC_0204</t>
+  </si>
+  <si>
+    <t>DEC_0205</t>
+  </si>
+  <si>
+    <t>DEC_0206</t>
+  </si>
+  <si>
+    <t>DEC_0207</t>
+  </si>
+  <si>
+    <t>DEC_0208</t>
+  </si>
+  <si>
+    <t>DEC_0209</t>
+  </si>
+  <si>
+    <t>DEC_0210</t>
+  </si>
+  <si>
+    <t>DEC_0211</t>
+  </si>
+  <si>
+    <t>DEC_0212</t>
+  </si>
+  <si>
+    <t>DEC_0213</t>
+  </si>
+  <si>
+    <t>DEC_0214</t>
+  </si>
+  <si>
+    <t>DEC_0215</t>
+  </si>
+  <si>
+    <t>DEC_0216</t>
+  </si>
+  <si>
+    <t>DEC_0217</t>
+  </si>
+  <si>
+    <t>DEC_0218</t>
+  </si>
+  <si>
+    <t>DEC_0219</t>
+  </si>
+  <si>
+    <t>DEC_0220</t>
   </si>
 </sst>
 </file>
@@ -853,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:J143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104:C117"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="G131" sqref="G131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4619,22 +4679,674 @@
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B118" s="4"/>
-      <c r="C118" s="4"/>
+      <c r="A118" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I118" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J118" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B119" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C119" s="4" t="s">
-        <v>3</v>
+      <c r="A119" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I119" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J119" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="B120" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C120" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I120" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J120" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I121" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J121" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I122" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J122" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I123" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J123" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I124" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J124" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A125" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I125" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J125" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H126" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I126" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J126" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I127" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J127" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H128" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I128" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J128" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I129" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J129" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H130" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I130" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J130" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H131" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I131" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J131" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A132" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G132" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H132" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I132" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J132" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H133" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I133" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J133" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A134" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H134" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I134" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J134" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A135" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H135" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I135" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J135" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A136" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H136" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I136" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J136" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A137" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H137" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I137" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J137" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B138" s="2"/>
+      <c r="C138" s="3"/>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B139" s="2"/>
+      <c r="C139" s="3"/>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B140" s="2"/>
+      <c r="C140" s="3"/>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B141" s="4"/>
+      <c r="C141" s="4"/>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B142" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B143" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C143" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agregan los scripts 0711/0715 a la clase Tests_MiPortal
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F6EDD8-DB48-454A-AFFB-3AAB9553E332}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B97721-29C0-419F-85D9-6DFC8A716720}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>18092588-0</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>plantilla dec qa</t>
+  </si>
+  <si>
+    <t>CVBNM</t>
+  </si>
+  <si>
+    <t>DEC_0711</t>
+  </si>
+  <si>
+    <t>DEC_0715</t>
   </si>
 </sst>
 </file>
@@ -418,7 +427,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,7 +435,7 @@
     <col min="1" max="1" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -501,6 +510,9 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -508,7 +520,7 @@
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
@@ -530,8 +542,36 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>

</xml_diff>

<commit_message>
Se crean los scripts 0716/0718/0720/0723/0724/0725/0726/0727 en la clase Tests_MiPortal
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B97721-29C0-419F-85D9-6DFC8A716720}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594BCFCA-F10D-4B1D-9F15-B8ACF7D80BC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="29">
   <si>
     <t>18092588-0</t>
   </si>
@@ -97,6 +97,30 @@
   </si>
   <si>
     <t>DEC_0715</t>
+  </si>
+  <si>
+    <t>DEC_0716</t>
+  </si>
+  <si>
+    <t>DEC_0718</t>
+  </si>
+  <si>
+    <t>DEC_0720</t>
+  </si>
+  <si>
+    <t>DEC_0723</t>
+  </si>
+  <si>
+    <t>DEC_0724</t>
+  </si>
+  <si>
+    <t>DEC_0725</t>
+  </si>
+  <si>
+    <t>DEC_0726</t>
+  </si>
+  <si>
+    <t>DEC_0727</t>
   </si>
 </sst>
 </file>
@@ -424,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A5" sqref="A5:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,30 +598,302 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="2"/>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="2"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agregan los scripts 0728/0729 a la clase Tests_MiPortal
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594BCFCA-F10D-4B1D-9F15-B8ACF7D80BC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51267F2-3BB9-4B2D-8DD9-F38E1823BA2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="34">
   <si>
     <t>18092588-0</t>
   </si>
@@ -121,6 +121,21 @@
   </si>
   <si>
     <t>DEC_0727</t>
+  </si>
+  <si>
+    <t>DEC_0728</t>
+  </si>
+  <si>
+    <t>DEC_0729</t>
+  </si>
+  <si>
+    <t>DEC_0730</t>
+  </si>
+  <si>
+    <t>DEC_0731</t>
+  </si>
+  <si>
+    <t>DEC_0732</t>
   </si>
 </sst>
 </file>
@@ -448,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -854,46 +869,194 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
+      <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
+      <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="4" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B22" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="3" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agregan los scripts 0730/0732/0733/0734/0735/0738/0740/0741/0744/0749/0752 a la clase Tests_MiPortal
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51267F2-3BB9-4B2D-8DD9-F38E1823BA2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3648AF7-C321-41B7-A46A-5A1F8FC5D073}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="59">
   <si>
     <t>18092588-0</t>
   </si>
@@ -136,6 +136,81 @@
   </si>
   <si>
     <t>DEC_0732</t>
+  </si>
+  <si>
+    <t>DEC_0733</t>
+  </si>
+  <si>
+    <t>DEC_0734</t>
+  </si>
+  <si>
+    <t>DEC_0735</t>
+  </si>
+  <si>
+    <t>DEC_0736</t>
+  </si>
+  <si>
+    <t>DEC_0737</t>
+  </si>
+  <si>
+    <t>DEC_0738</t>
+  </si>
+  <si>
+    <t>DEC_0739</t>
+  </si>
+  <si>
+    <t>DEC_0740</t>
+  </si>
+  <si>
+    <t>DEC_0741</t>
+  </si>
+  <si>
+    <t>DEC_0742</t>
+  </si>
+  <si>
+    <t>DEC_0743</t>
+  </si>
+  <si>
+    <t>DEC_0744</t>
+  </si>
+  <si>
+    <t>DEC_0745</t>
+  </si>
+  <si>
+    <t>DEC_0746</t>
+  </si>
+  <si>
+    <t>DEC_0747</t>
+  </si>
+  <si>
+    <t>DEC_0748</t>
+  </si>
+  <si>
+    <t>DEC_0749</t>
+  </si>
+  <si>
+    <t>DEC_0750</t>
+  </si>
+  <si>
+    <t>DEC_0751</t>
+  </si>
+  <si>
+    <t>DEC_0752</t>
+  </si>
+  <si>
+    <t>DEC_0753</t>
+  </si>
+  <si>
+    <t>DEC_0754</t>
+  </si>
+  <si>
+    <t>DEC_0755</t>
+  </si>
+  <si>
+    <t>DEC_0756</t>
+  </si>
+  <si>
+    <t>DEC_0757</t>
   </si>
 </sst>
 </file>
@@ -463,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1029,34 +1104,830 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
+      <c r="A19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
+      <c r="A20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="A21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="4" t="s">
+      <c r="A22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B43" s="2"/>
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B44" s="2"/>
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B46" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C46" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="3" t="s">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B47" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agrega Script 0753 a la clase Tests_MiPortal
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3648AF7-C321-41B7-A46A-5A1F8FC5D073}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E68F72-5013-4F0C-ADBA-71D63952B7C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="72">
   <si>
     <t>18092588-0</t>
   </si>
@@ -211,6 +211,45 @@
   </si>
   <si>
     <t>DEC_0757</t>
+  </si>
+  <si>
+    <t>DEC_0758</t>
+  </si>
+  <si>
+    <t>DEC_0759</t>
+  </si>
+  <si>
+    <t>DEC_0760</t>
+  </si>
+  <si>
+    <t>DEC_0761</t>
+  </si>
+  <si>
+    <t>DEC_0762</t>
+  </si>
+  <si>
+    <t>DEC_0763</t>
+  </si>
+  <si>
+    <t>DEC_0764</t>
+  </si>
+  <si>
+    <t>DEC_0765</t>
+  </si>
+  <si>
+    <t>DEC_0766</t>
+  </si>
+  <si>
+    <t>DEC_0767</t>
+  </si>
+  <si>
+    <t>DEC_0768</t>
+  </si>
+  <si>
+    <t>DEC_0769</t>
+  </si>
+  <si>
+    <t>DEC_0770</t>
   </si>
 </sst>
 </file>
@@ -538,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1904,30 +1943,446 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B43" s="2"/>
-      <c r="C43" s="3"/>
+      <c r="A43" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B44" s="2"/>
-      <c r="C44" s="3"/>
+      <c r="A44" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
+      <c r="A45" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B46" s="4" t="s">
+      <c r="A46" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B56" s="2"/>
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B57" s="2"/>
+      <c r="C57" s="3"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B59" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C59" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B47" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" s="3" t="s">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B60" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agregan los scripts 0768/0771/0775/0776/0779/0781/0782/0784/0785/0788 a la clase Tests_MiPortal
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E68F72-5013-4F0C-ADBA-71D63952B7C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71708FA5-19D6-47E3-8859-1BC55F9D8F04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22296" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="91">
   <si>
     <t>18092588-0</t>
   </si>
@@ -250,6 +250,63 @@
   </si>
   <si>
     <t>DEC_0770</t>
+  </si>
+  <si>
+    <t>DEC_0771</t>
+  </si>
+  <si>
+    <t>DEC_0772</t>
+  </si>
+  <si>
+    <t>DEC_0773</t>
+  </si>
+  <si>
+    <t>DEC_0774</t>
+  </si>
+  <si>
+    <t>DEC_0775</t>
+  </si>
+  <si>
+    <t>DEC_0776</t>
+  </si>
+  <si>
+    <t>DEC_0777</t>
+  </si>
+  <si>
+    <t>DEC_0778</t>
+  </si>
+  <si>
+    <t>DEC_0779</t>
+  </si>
+  <si>
+    <t>DEC_0780</t>
+  </si>
+  <si>
+    <t>DEC_0781</t>
+  </si>
+  <si>
+    <t>DEC_0782</t>
+  </si>
+  <si>
+    <t>DEC_0783</t>
+  </si>
+  <si>
+    <t>DEC_0784</t>
+  </si>
+  <si>
+    <t>DEC_0785</t>
+  </si>
+  <si>
+    <t>DEC_0786</t>
+  </si>
+  <si>
+    <t>DEC_0787</t>
+  </si>
+  <si>
+    <t>DEC_0788</t>
+  </si>
+  <si>
+    <t>DEC_0789</t>
   </si>
 </sst>
 </file>
@@ -577,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2359,30 +2416,646 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B56" s="2"/>
-      <c r="C56" s="3"/>
+      <c r="A56" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B57" s="2"/>
-      <c r="C57" s="3"/>
+      <c r="A57" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
+      <c r="A58" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B59" s="4" t="s">
+      <c r="A59" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B75" s="2"/>
+      <c r="C75" s="3"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B76" s="2"/>
+      <c r="C76" s="3"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B77" s="2"/>
+      <c r="C77" s="3"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B78" s="2"/>
+      <c r="C78" s="3"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B80" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C80" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B60" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C60" s="3" t="s">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B81" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agregan los scripts 0805 se debe terminar/0819/0820/0823 a la clase Tests_MiPortal
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8037B1AC-E30E-49CC-8BC6-4B11B68AE956}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD429D5E-812C-438C-9786-385ED34C1AC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22296" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="34">
   <si>
     <t>18092588-0</t>
   </si>
@@ -84,67 +84,58 @@
     <t>sebA$1357</t>
   </si>
   <si>
-    <t>DEC_0795</t>
-  </si>
-  <si>
-    <t>DEC_0796</t>
-  </si>
-  <si>
-    <t>DEC_0797</t>
-  </si>
-  <si>
-    <t>DEC_0798</t>
-  </si>
-  <si>
-    <t>DEC_0799</t>
-  </si>
-  <si>
-    <t>DEC_0800</t>
-  </si>
-  <si>
-    <t>DEC_0801</t>
-  </si>
-  <si>
-    <t>DEC_0802</t>
-  </si>
-  <si>
-    <t>DEC_0803</t>
-  </si>
-  <si>
-    <t>DEC_0804</t>
-  </si>
-  <si>
-    <t>DEC_0805</t>
-  </si>
-  <si>
-    <t>DEC_0806</t>
-  </si>
-  <si>
-    <t>DEC_0807</t>
-  </si>
-  <si>
-    <t>DEC_0808</t>
-  </si>
-  <si>
-    <t>DEC_0809</t>
-  </si>
-  <si>
-    <t>DEC_0810</t>
-  </si>
-  <si>
-    <t>DEC_0811</t>
-  </si>
-  <si>
-    <t>DEC_0812</t>
-  </si>
-  <si>
-    <t>DEC_0813</t>
-  </si>
-  <si>
-    <t>DEC_0814</t>
-  </si>
-  <si>
     <t>DEC_0815</t>
+  </si>
+  <si>
+    <t>DEC_0816</t>
+  </si>
+  <si>
+    <t>DEC_0817</t>
+  </si>
+  <si>
+    <t>DEC_0818</t>
+  </si>
+  <si>
+    <t>DEC_0819</t>
+  </si>
+  <si>
+    <t>DEC_0820</t>
+  </si>
+  <si>
+    <t>DEC_0821</t>
+  </si>
+  <si>
+    <t>DEC_0822</t>
+  </si>
+  <si>
+    <t>DEC_0823</t>
+  </si>
+  <si>
+    <t>DEC_0824</t>
+  </si>
+  <si>
+    <t>DEC_0825</t>
+  </si>
+  <si>
+    <t>DEC_0826</t>
+  </si>
+  <si>
+    <t>DEC_0827</t>
+  </si>
+  <si>
+    <t>DEC_0828</t>
+  </si>
+  <si>
+    <t>DEC_0829</t>
+  </si>
+  <si>
+    <t>DEC_0830</t>
+  </si>
+  <si>
+    <t>DEC_0831</t>
+  </si>
+  <si>
+    <t>DEC_0832</t>
   </si>
 </sst>
 </file>
@@ -472,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1102,142 +1093,38 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="2"/>
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-    </row>
-    <row r="30" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="4" t="s">
+    <row r="24" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B31" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="3" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Test 1100-1101 y del 1107-1123 de la clase Mis Documentos
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura Andrade\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8E28D6-0DC2-448E-8496-311E0D441E0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A376EA20-ABFE-48CF-AB73-4DD24E05F6DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1689" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1899" uniqueCount="201">
   <si>
     <t>18092588-0</t>
   </si>
@@ -486,9 +486,6 @@
     <t>DEC_1090</t>
   </si>
   <si>
-    <t>DEC_1091</t>
-  </si>
-  <si>
     <t>DEC_0728</t>
   </si>
   <si>
@@ -595,6 +592,51 @@
   </si>
   <si>
     <t>DEC_1099</t>
+  </si>
+  <si>
+    <t>DEC_1100</t>
+  </si>
+  <si>
+    <t>DEC_1101</t>
+  </si>
+  <si>
+    <t>DEC_1103</t>
+  </si>
+  <si>
+    <t>DEC_1104</t>
+  </si>
+  <si>
+    <t>DEC_1105</t>
+  </si>
+  <si>
+    <t>DEC_1107</t>
+  </si>
+  <si>
+    <t>DEC_1108</t>
+  </si>
+  <si>
+    <t>DEC_1110</t>
+  </si>
+  <si>
+    <t>DEC_1112</t>
+  </si>
+  <si>
+    <t>DEC_1113</t>
+  </si>
+  <si>
+    <t>DEC_1114</t>
+  </si>
+  <si>
+    <t>DEC_1115</t>
+  </si>
+  <si>
+    <t>DEC_1117</t>
+  </si>
+  <si>
+    <t>DEC_1119</t>
+  </si>
+  <si>
+    <t>DEC_1120</t>
   </si>
 </sst>
 </file>
@@ -929,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O148"/>
+  <dimension ref="A1:O162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2315,7 +2357,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>0</v>
@@ -2347,7 +2389,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>0</v>
@@ -2379,7 +2421,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>0</v>
@@ -2411,7 +2453,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>0</v>
@@ -2443,7 +2485,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>0</v>
@@ -2475,7 +2517,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>0</v>
@@ -2507,7 +2549,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>0</v>
@@ -2539,7 +2581,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>0</v>
@@ -2571,7 +2613,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>0</v>
@@ -2603,7 +2645,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>0</v>
@@ -2635,7 +2677,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>0</v>
@@ -2667,7 +2709,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>0</v>
@@ -2699,7 +2741,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>0</v>
@@ -2731,7 +2773,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>0</v>
@@ -2763,7 +2805,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>0</v>
@@ -2795,7 +2837,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>0</v>
@@ -2827,7 +2869,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>0</v>
@@ -2859,7 +2901,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>0</v>
@@ -2891,7 +2933,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>0</v>
@@ -2923,7 +2965,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>0</v>
@@ -2955,7 +2997,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>0</v>
@@ -2987,7 +3029,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>0</v>
@@ -3019,7 +3061,7 @@
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>0</v>
@@ -3051,7 +3093,7 @@
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>0</v>
@@ -3083,7 +3125,7 @@
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>0</v>
@@ -3115,7 +3157,7 @@
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>0</v>
@@ -3147,7 +3189,7 @@
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>0</v>
@@ -3179,7 +3221,7 @@
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>0</v>
@@ -3211,7 +3253,7 @@
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>0</v>
@@ -3243,7 +3285,7 @@
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>0</v>
@@ -4168,7 +4210,7 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>2</v>
@@ -4365,7 +4407,7 @@
         <v>64</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>17</v>
+        <v>146</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>16</v>
@@ -4459,7 +4501,7 @@
         <v>64</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>16</v>
@@ -4497,7 +4539,7 @@
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>87</v>
+        <v>187</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>2</v>
@@ -4543,8 +4585,8 @@
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A100" s="5" t="s">
-        <v>65</v>
+      <c r="A100" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>2</v>
@@ -4574,24 +4616,24 @@
         <v>16</v>
       </c>
       <c r="K100" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L100" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M100" s="1" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="N100" s="1" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="O100" s="1" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>72</v>
+        <v>189</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>2</v>
@@ -4621,24 +4663,24 @@
         <v>16</v>
       </c>
       <c r="K101" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L101" s="1" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="M101" s="1" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="N101" s="1" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="O101" s="1" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>74</v>
+        <v>190</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>2</v>
@@ -4668,24 +4710,24 @@
         <v>16</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L102" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M102" s="1" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="N102" s="1" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="O102" s="1" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>75</v>
+        <v>191</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>2</v>
@@ -4715,24 +4757,24 @@
         <v>16</v>
       </c>
       <c r="K103" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L103" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M103" s="1" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="N103" s="1" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="O103" s="1" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>78</v>
+        <v>192</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>2</v>
@@ -4762,24 +4804,24 @@
         <v>16</v>
       </c>
       <c r="K104" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L104" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M104" s="1" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="N104" s="1" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="O104" s="1" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>91</v>
+        <v>193</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>2</v>
@@ -4826,7 +4868,7 @@
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>98</v>
+        <v>194</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>2</v>
@@ -4835,7 +4877,7 @@
         <v>64</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>17</v>
+        <v>146</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>16</v>
@@ -4873,7 +4915,7 @@
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>89</v>
+        <v>195</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>2</v>
@@ -4882,7 +4924,7 @@
         <v>64</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>17</v>
+        <v>146</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>16</v>
@@ -4920,7 +4962,7 @@
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>90</v>
+        <v>196</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>2</v>
@@ -4929,7 +4971,7 @@
         <v>64</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>16</v>
@@ -4967,7 +5009,7 @@
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>92</v>
+        <v>197</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>2</v>
@@ -5014,7 +5056,7 @@
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>88</v>
+        <v>198</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>2</v>
@@ -5061,7 +5103,7 @@
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>80</v>
+        <v>199</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>2</v>
@@ -5108,7 +5150,7 @@
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>82</v>
+        <v>200</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>2</v>
@@ -5155,7 +5197,7 @@
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>2</v>
@@ -5185,10 +5227,10 @@
         <v>16</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L113" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M113" s="1" t="s">
         <v>16</v>
@@ -5201,8 +5243,8 @@
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>83</v>
+      <c r="A114" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>2</v>
@@ -5238,18 +5280,18 @@
         <v>2</v>
       </c>
       <c r="M114" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="N114" s="1" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="O114" s="1" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>2</v>
@@ -5282,21 +5324,21 @@
         <v>77</v>
       </c>
       <c r="L115" s="1" t="s">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="M115" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="N115" s="1" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="O115" s="1" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>2</v>
@@ -5332,18 +5374,18 @@
         <v>2</v>
       </c>
       <c r="M116" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="N116" s="1" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="O116" s="1" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>2</v>
@@ -5373,24 +5415,24 @@
         <v>16</v>
       </c>
       <c r="K117" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L117" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="M117" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="N117" s="1" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="O117" s="1" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="B118" s="4" t="s">
         <v>2</v>
@@ -5426,18 +5468,18 @@
         <v>2</v>
       </c>
       <c r="M118" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="N118" s="1" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="O118" s="1" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>2</v>
@@ -5467,10 +5509,10 @@
         <v>16</v>
       </c>
       <c r="K119" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L119" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M119" s="1" t="s">
         <v>16</v>
@@ -5484,7 +5526,7 @@
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>2</v>
@@ -5514,10 +5556,10 @@
         <v>16</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L120" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M120" s="1" t="s">
         <v>16</v>
@@ -5531,7 +5573,7 @@
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>2</v>
@@ -5561,7 +5603,7 @@
         <v>16</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L121" s="1" t="s">
         <v>16</v>
@@ -5578,7 +5620,7 @@
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>2</v>
@@ -5608,10 +5650,10 @@
         <v>16</v>
       </c>
       <c r="K122" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L122" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M122" s="1" t="s">
         <v>16</v>
@@ -5625,7 +5667,7 @@
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B123" s="4" t="s">
         <v>2</v>
@@ -5655,10 +5697,10 @@
         <v>16</v>
       </c>
       <c r="K123" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L123" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M123" s="1" t="s">
         <v>16</v>
@@ -5672,7 +5714,7 @@
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="B124" s="4" t="s">
         <v>2</v>
@@ -5702,10 +5744,10 @@
         <v>16</v>
       </c>
       <c r="K124" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L124" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M124" s="1" t="s">
         <v>16</v>
@@ -5719,7 +5761,7 @@
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B125" s="4" t="s">
         <v>2</v>
@@ -5766,7 +5808,7 @@
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B126" s="4" t="s">
         <v>2</v>
@@ -5813,7 +5855,7 @@
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B127" s="4" t="s">
         <v>2</v>
@@ -5843,7 +5885,7 @@
         <v>16</v>
       </c>
       <c r="K127" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L127" s="1" t="s">
         <v>2</v>
@@ -5860,7 +5902,7 @@
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="B128" s="4" t="s">
         <v>2</v>
@@ -5890,7 +5932,7 @@
         <v>16</v>
       </c>
       <c r="K128" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L128" s="1" t="s">
         <v>2</v>
@@ -5907,7 +5949,7 @@
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B129" s="4" t="s">
         <v>2</v>
@@ -5937,7 +5979,7 @@
         <v>16</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L129" s="1" t="s">
         <v>2</v>
@@ -5954,7 +5996,7 @@
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B130" s="4" t="s">
         <v>2</v>
@@ -5984,7 +6026,7 @@
         <v>16</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L130" s="1" t="s">
         <v>2</v>
@@ -6001,7 +6043,7 @@
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B131" s="4" t="s">
         <v>2</v>
@@ -6034,7 +6076,7 @@
         <v>16</v>
       </c>
       <c r="L131" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M131" s="1" t="s">
         <v>16</v>
@@ -6048,7 +6090,7 @@
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B132" s="4" t="s">
         <v>2</v>
@@ -6078,7 +6120,7 @@
         <v>16</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L132" s="1" t="s">
         <v>2</v>
@@ -6095,7 +6137,7 @@
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B133" s="4" t="s">
         <v>2</v>
@@ -6125,10 +6167,10 @@
         <v>16</v>
       </c>
       <c r="K133" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L133" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="M133" s="1" t="s">
         <v>16</v>
@@ -6142,7 +6184,7 @@
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B134" s="4" t="s">
         <v>2</v>
@@ -6172,10 +6214,10 @@
         <v>16</v>
       </c>
       <c r="K134" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L134" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="M134" s="1" t="s">
         <v>16</v>
@@ -6189,7 +6231,7 @@
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B135" s="4" t="s">
         <v>2</v>
@@ -6219,7 +6261,7 @@
         <v>16</v>
       </c>
       <c r="K135" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L135" s="1" t="s">
         <v>16</v>
@@ -6236,104 +6278,762 @@
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H136" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I136" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J136" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K136" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L136" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M136" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N136" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O136" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H137" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I137" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J137" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K137" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L137" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M137" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N137" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O137" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H138" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I138" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J138" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K138" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L138" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M138" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N138" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O138" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H139" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I139" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J139" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K139" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L139" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M139" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N139" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O139" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G140" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H140" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I140" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J140" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K140" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L140" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M140" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N140" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O140" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H141" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I141" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J141" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K141" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L141" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M141" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N141" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O141" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G142" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H142" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I142" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J142" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K142" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L142" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M142" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N142" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O142" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C143" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H143" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I143" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J143" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K143" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L143" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M143" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N143" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O143" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C144" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H144" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I144" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J144" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K144" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L144" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M144" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N144" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O144" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H145" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I145" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J145" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K145" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L145" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M145" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N145" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O145" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B146" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G146" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H146" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I146" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J146" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K146" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L146" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M146" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N146" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O146" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C147" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H147" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I147" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J147" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K147" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L147" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M147" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N147" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O147" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B148" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C148" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G148" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H148" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I148" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J148" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K148" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L148" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M148" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N148" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O148" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H149" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I149" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J149" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K149" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L149" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M149" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N149" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O149" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B136" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C136" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F136" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G136" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H136" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I136" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J136" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K136" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L136" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M136" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N136" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O136" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B137" s="4"/>
-      <c r="C137" s="4"/>
-    </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B138" s="4"/>
-      <c r="C138" s="4"/>
-    </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B139" s="4"/>
-      <c r="C139" s="4"/>
-    </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B140" s="4"/>
-      <c r="C140" s="4"/>
-    </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B141" s="4"/>
-      <c r="C141" s="4"/>
-    </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B142" s="4"/>
-      <c r="C142" s="4"/>
-    </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B143" s="4"/>
-      <c r="C143" s="4"/>
-    </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B144" s="4"/>
-      <c r="C144" s="4"/>
-    </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B145" s="4"/>
-      <c r="C145" s="4"/>
-    </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B146" s="4"/>
-      <c r="C146" s="4"/>
-    </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B147" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C147" s="4" t="s">
+      <c r="B150" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C150" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G150" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H150" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I150" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J150" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K150" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L150" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M150" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N150" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O150" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B151" s="4"/>
+      <c r="C151" s="4"/>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B152" s="4"/>
+      <c r="C152" s="4"/>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B153" s="4"/>
+      <c r="C153" s="4"/>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B154" s="4"/>
+      <c r="C154" s="4"/>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B155" s="4"/>
+      <c r="C155" s="4"/>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B156" s="4"/>
+      <c r="C156" s="4"/>
+    </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B157" s="4"/>
+      <c r="C157" s="4"/>
+    </row>
+    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B158" s="4"/>
+      <c r="C158" s="4"/>
+    </row>
+    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B159" s="4"/>
+      <c r="C159" s="4"/>
+    </row>
+    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B160" s="4"/>
+      <c r="C160" s="4"/>
+    </row>
+    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B161" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C161" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B148" s="2" t="s">
+    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B162" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C148" s="3" t="s">
+      <c r="C162" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test 1103-1105 y del 1127-1131 de la clase Mis Documentos
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura Andrade\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A376EA20-ABFE-48CF-AB73-4DD24E05F6DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E197B13-6136-4DB8-A876-3CA983BFAB9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1899" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1974" uniqueCount="206">
   <si>
     <t>18092588-0</t>
   </si>
@@ -637,6 +637,21 @@
   </si>
   <si>
     <t>DEC_1120</t>
+  </si>
+  <si>
+    <t>DEC_1122</t>
+  </si>
+  <si>
+    <t>DEC_1123</t>
+  </si>
+  <si>
+    <t>DEC_1127</t>
+  </si>
+  <si>
+    <t>DEC_1128</t>
+  </si>
+  <si>
+    <t>DEC_1131</t>
   </si>
 </sst>
 </file>
@@ -971,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O162"/>
+  <dimension ref="A1:O167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5197,7 +5212,7 @@
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>87</v>
+        <v>201</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>2</v>
@@ -5243,8 +5258,8 @@
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A114" s="5" t="s">
-        <v>65</v>
+      <c r="A114" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>2</v>
@@ -5274,24 +5289,24 @@
         <v>16</v>
       </c>
       <c r="K114" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L114" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M114" s="1" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="N114" s="1" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="O114" s="1" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>72</v>
+        <v>203</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>2</v>
@@ -5321,24 +5336,24 @@
         <v>16</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L115" s="1" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="M115" s="1" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="N115" s="1" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="O115" s="1" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>74</v>
+        <v>204</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>2</v>
@@ -5368,24 +5383,24 @@
         <v>16</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L116" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M116" s="1" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="N116" s="1" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="O116" s="1" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>75</v>
+        <v>205</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>2</v>
@@ -5415,24 +5430,24 @@
         <v>16</v>
       </c>
       <c r="K117" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L117" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M117" s="1" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="N117" s="1" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="O117" s="1" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B118" s="4" t="s">
         <v>2</v>
@@ -5462,71 +5477,71 @@
         <v>16</v>
       </c>
       <c r="K118" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L118" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M118" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N118" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O118" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A119" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I119" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J119" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K119" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="L118" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M118" s="1" t="s">
+      <c r="L119" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M119" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="N118" s="1" t="s">
+      <c r="N119" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="O118" s="1" t="s">
+      <c r="O119" s="1" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B119" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C119" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H119" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I119" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J119" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K119" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L119" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M119" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N119" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O119" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>2</v>
@@ -5556,24 +5571,24 @@
         <v>16</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L120" s="1" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="M120" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="N120" s="1" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="O120" s="1" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>2</v>
@@ -5603,24 +5618,24 @@
         <v>16</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L121" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="M121" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="N121" s="1" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="O121" s="1" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>2</v>
@@ -5650,24 +5665,24 @@
         <v>16</v>
       </c>
       <c r="K122" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L122" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="M122" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="N122" s="1" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="O122" s="1" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B123" s="4" t="s">
         <v>2</v>
@@ -5697,24 +5712,24 @@
         <v>16</v>
       </c>
       <c r="K123" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L123" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="M123" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="N123" s="1" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="O123" s="1" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B124" s="4" t="s">
         <v>2</v>
@@ -5761,7 +5776,7 @@
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B125" s="4" t="s">
         <v>2</v>
@@ -5808,7 +5823,7 @@
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B126" s="4" t="s">
         <v>2</v>
@@ -5855,7 +5870,7 @@
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B127" s="4" t="s">
         <v>2</v>
@@ -5885,10 +5900,10 @@
         <v>16</v>
       </c>
       <c r="K127" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L127" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M127" s="1" t="s">
         <v>16</v>
@@ -5902,7 +5917,7 @@
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B128" s="4" t="s">
         <v>2</v>
@@ -5932,10 +5947,10 @@
         <v>16</v>
       </c>
       <c r="K128" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L128" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M128" s="1" t="s">
         <v>16</v>
@@ -5949,7 +5964,7 @@
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B129" s="4" t="s">
         <v>2</v>
@@ -5979,10 +5994,10 @@
         <v>16</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L129" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M129" s="1" t="s">
         <v>16</v>
@@ -5996,7 +6011,7 @@
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B130" s="4" t="s">
         <v>2</v>
@@ -6026,10 +6041,10 @@
         <v>16</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L130" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M130" s="1" t="s">
         <v>16</v>
@@ -6043,7 +6058,7 @@
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="B131" s="4" t="s">
         <v>2</v>
@@ -6090,7 +6105,7 @@
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B132" s="4" t="s">
         <v>2</v>
@@ -6137,7 +6152,7 @@
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B133" s="4" t="s">
         <v>2</v>
@@ -6184,7 +6199,7 @@
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B134" s="4" t="s">
         <v>2</v>
@@ -6231,7 +6246,7 @@
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B135" s="4" t="s">
         <v>2</v>
@@ -6264,7 +6279,7 @@
         <v>77</v>
       </c>
       <c r="L135" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="M135" s="1" t="s">
         <v>16</v>
@@ -6278,7 +6293,7 @@
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B136" s="4" t="s">
         <v>2</v>
@@ -6308,10 +6323,10 @@
         <v>16</v>
       </c>
       <c r="K136" s="1" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="L136" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M136" s="1" t="s">
         <v>16</v>
@@ -6325,7 +6340,7 @@
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B137" s="4" t="s">
         <v>2</v>
@@ -6372,7 +6387,7 @@
     </row>
     <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B138" s="4" t="s">
         <v>2</v>
@@ -6419,7 +6434,7 @@
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="B139" s="4" t="s">
         <v>2</v>
@@ -6449,10 +6464,10 @@
         <v>16</v>
       </c>
       <c r="K139" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L139" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="M139" s="1" t="s">
         <v>16</v>
@@ -6466,7 +6481,7 @@
     </row>
     <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B140" s="4" t="s">
         <v>2</v>
@@ -6496,7 +6511,7 @@
         <v>16</v>
       </c>
       <c r="K140" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L140" s="1" t="s">
         <v>16</v>
@@ -6513,7 +6528,7 @@
     </row>
     <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="B141" s="4" t="s">
         <v>2</v>
@@ -6543,7 +6558,7 @@
         <v>16</v>
       </c>
       <c r="K141" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L141" s="1" t="s">
         <v>2</v>
@@ -6560,7 +6575,7 @@
     </row>
     <row r="142" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B142" s="4" t="s">
         <v>2</v>
@@ -6590,7 +6605,7 @@
         <v>16</v>
       </c>
       <c r="K142" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L142" s="1" t="s">
         <v>2</v>
@@ -6607,7 +6622,7 @@
     </row>
     <row r="143" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B143" s="4" t="s">
         <v>2</v>
@@ -6637,7 +6652,7 @@
         <v>16</v>
       </c>
       <c r="K143" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L143" s="1" t="s">
         <v>2</v>
@@ -6654,7 +6669,7 @@
     </row>
     <row r="144" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="B144" s="4" t="s">
         <v>2</v>
@@ -6687,7 +6702,7 @@
         <v>16</v>
       </c>
       <c r="L144" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M144" s="1" t="s">
         <v>16</v>
@@ -6701,7 +6716,7 @@
     </row>
     <row r="145" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="B145" s="4" t="s">
         <v>2</v>
@@ -6734,7 +6749,7 @@
         <v>16</v>
       </c>
       <c r="L145" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M145" s="1" t="s">
         <v>16</v>
@@ -6748,7 +6763,7 @@
     </row>
     <row r="146" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="B146" s="4" t="s">
         <v>2</v>
@@ -6795,7 +6810,7 @@
     </row>
     <row r="147" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B147" s="4" t="s">
         <v>2</v>
@@ -6828,7 +6843,7 @@
         <v>16</v>
       </c>
       <c r="L147" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="M147" s="1" t="s">
         <v>16</v>
@@ -6842,7 +6857,7 @@
     </row>
     <row r="148" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B148" s="4" t="s">
         <v>2</v>
@@ -6875,7 +6890,7 @@
         <v>16</v>
       </c>
       <c r="L148" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="M148" s="1" t="s">
         <v>16</v>
@@ -6889,7 +6904,7 @@
     </row>
     <row r="149" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B149" s="4" t="s">
         <v>2</v>
@@ -6922,7 +6937,7 @@
         <v>16</v>
       </c>
       <c r="L149" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="M149" s="1" t="s">
         <v>16</v>
@@ -6936,70 +6951,285 @@
     </row>
     <row r="150" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B150" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C150" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G150" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H150" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I150" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J150" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K150" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L150" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M150" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N150" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O150" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B151" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C151" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H151" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I151" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J151" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K151" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L151" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M151" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N151" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O151" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B152" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C152" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G152" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H152" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I152" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J152" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K152" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L152" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M152" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N152" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O152" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B153" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C153" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G153" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H153" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I153" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J153" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K153" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L153" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M153" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N153" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O153" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C154" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G154" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H154" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I154" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J154" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K154" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L154" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M154" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N154" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O154" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B150" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C150" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F150" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G150" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H150" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I150" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J150" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K150" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L150" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M150" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N150" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O150" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B151" s="4"/>
-      <c r="C151" s="4"/>
-    </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B152" s="4"/>
-      <c r="C152" s="4"/>
-    </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B153" s="4"/>
-      <c r="C153" s="4"/>
-    </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B154" s="4"/>
-      <c r="C154" s="4"/>
-    </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B155" s="4"/>
-      <c r="C155" s="4"/>
+      <c r="B155" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C155" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G155" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H155" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I155" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J155" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K155" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L155" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M155" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N155" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O155" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="156" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B156" s="4"/>
@@ -7022,18 +7252,38 @@
       <c r="C160" s="4"/>
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B161" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C161" s="4" t="s">
+      <c r="B161" s="4"/>
+      <c r="C161" s="4"/>
+    </row>
+    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B162" s="4"/>
+      <c r="C162" s="4"/>
+    </row>
+    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B163" s="4"/>
+      <c r="C163" s="4"/>
+    </row>
+    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B164" s="4"/>
+      <c r="C164" s="4"/>
+    </row>
+    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B165" s="4"/>
+      <c r="C165" s="4"/>
+    </row>
+    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B166" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C166" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B162" s="2" t="s">
+    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B167" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C162" s="3" t="s">
+      <c r="C167" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agregan los scripts 0837/0838/0839/0841/0842/0843 a la clase Tests_MiPortal
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52BBD3AF-CB58-403A-BE66-894CCA57F026}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D2A81C-472D-4AB2-82DB-EDA2B7A6BE92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22296" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="72">
   <si>
     <t>18092588-0</t>
   </si>
@@ -172,6 +172,84 @@
   </si>
   <si>
     <t>DEC_0844</t>
+  </si>
+  <si>
+    <t>DEC_0845</t>
+  </si>
+  <si>
+    <t>DEC_0846</t>
+  </si>
+  <si>
+    <t>DEC_0847</t>
+  </si>
+  <si>
+    <t>DEC_0848</t>
+  </si>
+  <si>
+    <t>DEC_0849</t>
+  </si>
+  <si>
+    <t>DEC_0850</t>
+  </si>
+  <si>
+    <t>DEC_0851</t>
+  </si>
+  <si>
+    <t>DEC_0852</t>
+  </si>
+  <si>
+    <t>DEC_0853</t>
+  </si>
+  <si>
+    <t>DEC_0854</t>
+  </si>
+  <si>
+    <t>DEC_0855</t>
+  </si>
+  <si>
+    <t>DEC_0856</t>
+  </si>
+  <si>
+    <t>DEC_0857</t>
+  </si>
+  <si>
+    <t>DEC_0858</t>
+  </si>
+  <si>
+    <t>DEC_0859</t>
+  </si>
+  <si>
+    <t>DEC_0860</t>
+  </si>
+  <si>
+    <t>DEC_0861</t>
+  </si>
+  <si>
+    <t>DEC_0862</t>
+  </si>
+  <si>
+    <t>DEC_0863</t>
+  </si>
+  <si>
+    <t>DEC_0864</t>
+  </si>
+  <si>
+    <t>DEC_0865</t>
+  </si>
+  <si>
+    <t>DEC_0866</t>
+  </si>
+  <si>
+    <t>DEC_0867</t>
+  </si>
+  <si>
+    <t>DEC_0868</t>
+  </si>
+  <si>
+    <t>DEC_0869</t>
+  </si>
+  <si>
+    <t>DEC_0870</t>
   </si>
 </sst>
 </file>
@@ -499,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1513,30 +1591,858 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" s="2"/>
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="2:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-    </row>
-    <row r="35" spans="2:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="4" t="s">
+      <c r="A32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B58" s="2"/>
+      <c r="C58" s="3"/>
+    </row>
+    <row r="59" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+    </row>
+    <row r="60" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C60" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B36" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="3" t="s">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B61" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tests 867 869 870 871 y 872 Mi Portal 2
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estef\eclipse-workspace\Dec5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Verity-Usuario\eclipse-workspace\AceptaDec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D2A81C-472D-4AB2-82DB-EDA2B7A6BE92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74674E6E-C394-479E-B26C-7BBE9E258F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22296" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="74">
   <si>
     <t>18092588-0</t>
   </si>
@@ -250,6 +250,12 @@
   </si>
   <si>
     <t>DEC_0870</t>
+  </si>
+  <si>
+    <t>DEC_0871</t>
+  </si>
+  <si>
+    <t>DEC_0872</t>
   </si>
 </sst>
 </file>
@@ -577,28 +583,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="10" max="10" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -630,7 +635,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -662,7 +667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -694,7 +699,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -726,7 +731,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -758,7 +763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -790,7 +795,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -822,7 +827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -854,7 +859,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -886,7 +891,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -918,7 +923,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -950,7 +955,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -982,7 +987,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -1014,7 +1019,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -1046,7 +1051,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -1078,7 +1083,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -1110,7 +1115,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1142,7 +1147,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -1174,7 +1179,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
@@ -1206,7 +1211,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
@@ -1238,7 +1243,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>35</v>
       </c>
@@ -1270,7 +1275,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
@@ -1302,7 +1307,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>37</v>
       </c>
@@ -1334,7 +1339,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
@@ -1366,7 +1371,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
@@ -1398,7 +1403,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>40</v>
       </c>
@@ -1430,7 +1435,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
@@ -1462,7 +1467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>42</v>
       </c>
@@ -1494,7 +1499,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>43</v>
       </c>
@@ -1526,7 +1531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>44</v>
       </c>
@@ -1558,7 +1563,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>45</v>
       </c>
@@ -1590,7 +1595,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>46</v>
       </c>
@@ -1622,7 +1627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>47</v>
       </c>
@@ -1654,7 +1659,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>48</v>
       </c>
@@ -1686,7 +1691,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>49</v>
       </c>
@@ -1718,7 +1723,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>50</v>
       </c>
@@ -1750,7 +1755,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>51</v>
       </c>
@@ -1782,7 +1787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>52</v>
       </c>
@@ -1814,7 +1819,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>53</v>
       </c>
@@ -1846,7 +1851,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>54</v>
       </c>
@@ -1878,7 +1883,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>55</v>
       </c>
@@ -1910,7 +1915,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>56</v>
       </c>
@@ -1942,7 +1947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>57</v>
       </c>
@@ -1974,7 +1979,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>58</v>
       </c>
@@ -2006,7 +2011,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>59</v>
       </c>
@@ -2038,7 +2043,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>60</v>
       </c>
@@ -2070,7 +2075,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>61</v>
       </c>
@@ -2102,7 +2107,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>62</v>
       </c>
@@ -2134,7 +2139,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>63</v>
       </c>
@@ -2166,7 +2171,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>64</v>
       </c>
@@ -2198,7 +2203,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>65</v>
       </c>
@@ -2230,7 +2235,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>66</v>
       </c>
@@ -2262,7 +2267,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>67</v>
       </c>
@@ -2294,7 +2299,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>68</v>
       </c>
@@ -2326,7 +2331,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>69</v>
       </c>
@@ -2358,7 +2363,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>70</v>
       </c>
@@ -2390,7 +2395,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>71</v>
       </c>
@@ -2422,27 +2427,95 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B58" s="2"/>
-      <c r="C58" s="3"/>
-    </row>
-    <row r="59" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-    </row>
-    <row r="60" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="4" t="s">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B60" s="2"/>
+      <c r="C60" s="3"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B61" s="2"/>
+      <c r="C61" s="3"/>
+    </row>
+    <row r="62" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+    </row>
+    <row r="63" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C63" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B61" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C61" s="3" t="s">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B64" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tests 874 876 877 879 880 884 Clase MiPortal2
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Verity-Usuario\eclipse-workspace\AceptaDec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74674E6E-C394-479E-B26C-7BBE9E258F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF8A9D3-5602-430B-A46D-B6F9A8608330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="84">
   <si>
     <t>18092588-0</t>
   </si>
@@ -256,6 +256,36 @@
   </si>
   <si>
     <t>DEC_0872</t>
+  </si>
+  <si>
+    <t>DEC_1139</t>
+  </si>
+  <si>
+    <t>Verity3.0</t>
+  </si>
+  <si>
+    <t>verity</t>
+  </si>
+  <si>
+    <t>DEC_0874</t>
+  </si>
+  <si>
+    <t>DEC_0876</t>
+  </si>
+  <si>
+    <t>DEC_0877</t>
+  </si>
+  <si>
+    <t>DEC_0879</t>
+  </si>
+  <si>
+    <t>DEC_0880</t>
+  </si>
+  <si>
+    <t>DEC_0884</t>
+  </si>
+  <si>
+    <t>DEC_0885</t>
   </si>
 </sst>
 </file>
@@ -297,11 +327,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -583,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2491,31 +2523,302 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B60" s="2"/>
-      <c r="C60" s="3"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B61" s="2"/>
-      <c r="C61" s="3"/>
-    </row>
-    <row r="62" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-    </row>
-    <row r="63" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
+    <row r="60" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I66" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J66" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="2"/>
+      <c r="C67" s="3"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B68" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C68" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O68" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B69" s="2"/>
+      <c r="C69" s="3"/>
+    </row>
+    <row r="70" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+    </row>
+    <row r="71" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B64" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C64" s="3" t="s">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B72" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tests 888, 890, 891, 893, 894, 896, 897, 899, 900, 903, 904, 905, 907, 908, 909, 912, 915, 916, 917 y 918 clase MiPortal2
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Verity-Usuario\eclipse-workspace\AceptaDec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF8A9D3-5602-430B-A46D-B6F9A8608330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A806B8-4E5F-4300-A366-3F138070A50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="110">
   <si>
     <t>18092588-0</t>
   </si>
@@ -286,6 +286,84 @@
   </si>
   <si>
     <t>DEC_0885</t>
+  </si>
+  <si>
+    <t>DEC_0888</t>
+  </si>
+  <si>
+    <t>DEC_0890</t>
+  </si>
+  <si>
+    <t>DEC_0891</t>
+  </si>
+  <si>
+    <t>DEC_0893</t>
+  </si>
+  <si>
+    <t>DEC_0894</t>
+  </si>
+  <si>
+    <t>DEC_0896</t>
+  </si>
+  <si>
+    <t>DEC_0897</t>
+  </si>
+  <si>
+    <t>DEC_0787</t>
+  </si>
+  <si>
+    <t>DEC_0899</t>
+  </si>
+  <si>
+    <t>DEC_0900</t>
+  </si>
+  <si>
+    <t>DEC_0903</t>
+  </si>
+  <si>
+    <t>DEC_0904</t>
+  </si>
+  <si>
+    <t>DEC_0905</t>
+  </si>
+  <si>
+    <t>DEC_0907</t>
+  </si>
+  <si>
+    <t>DEC_0908</t>
+  </si>
+  <si>
+    <t>DEC_0909</t>
+  </si>
+  <si>
+    <t>DEC_0912</t>
+  </si>
+  <si>
+    <t>DEC_0913</t>
+  </si>
+  <si>
+    <t>DEC_0914</t>
+  </si>
+  <si>
+    <t>DEC_0915</t>
+  </si>
+  <si>
+    <t>DEC_0916</t>
+  </si>
+  <si>
+    <t>DEC_0917</t>
+  </si>
+  <si>
+    <t>DEC_0918</t>
+  </si>
+  <si>
+    <t>DEC_0919</t>
+  </si>
+  <si>
+    <t>DEC_0921</t>
+  </si>
+  <si>
+    <t>DEC_0922</t>
   </si>
 </sst>
 </file>
@@ -615,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O72"/>
+  <dimension ref="A1:O100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2683,7 +2761,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>82</v>
       </c>
@@ -2715,7 +2793,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>83</v>
       </c>
@@ -2747,78 +2825,918 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="2"/>
-      <c r="C67" s="3"/>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I67" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J67" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J68" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J69" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I70" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J70" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J71" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H72" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I72" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J72" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J73" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I74" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J74" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H75" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I75" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J75" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I76" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J76" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H77" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I77" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J77" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I78" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J78" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I79" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J79" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I80" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J80" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H81" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I81" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J81" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H82" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I82" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J82" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H83" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I83" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J83" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H84" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I84" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J84" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H85" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I85" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J85" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G86" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H86" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I86" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J86" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G87" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H87" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I87" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J87" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J88" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H89" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I89" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J89" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G90" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H90" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I90" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J90" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G91" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H91" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I91" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J91" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G92" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H92" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I92" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J92" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="2"/>
+      <c r="C93" s="3"/>
+    </row>
+    <row r="94" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="2"/>
+      <c r="C94" s="3"/>
+    </row>
+    <row r="95" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="2"/>
+      <c r="C95" s="3"/>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B96" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C96" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D96" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E68" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H68" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I68" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J68" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K68" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="L68" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M68" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="N68" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="O68" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="2"/>
-      <c r="C69" s="3"/>
-    </row>
-    <row r="70" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-    </row>
-    <row r="71" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="4" t="s">
+      <c r="E96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O96" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B97" s="2"/>
+      <c r="C97" s="3"/>
+    </row>
+    <row r="98" spans="2:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+    </row>
+    <row r="99" spans="2:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C99" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C72" s="3" t="s">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B100" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C100" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
919 al 965 clase MiPortal2
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Verity-Usuario\eclipse-workspace\AceptaDec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A806B8-4E5F-4300-A366-3F138070A50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348A0FA4-548F-4729-A05F-3F90B8E672ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="148">
   <si>
     <t>18092588-0</t>
   </si>
@@ -364,6 +364,120 @@
   </si>
   <si>
     <t>DEC_0922</t>
+  </si>
+  <si>
+    <t>DEC_0923</t>
+  </si>
+  <si>
+    <t>DEC_0924</t>
+  </si>
+  <si>
+    <t>DEC_0927</t>
+  </si>
+  <si>
+    <t>DEC_0928</t>
+  </si>
+  <si>
+    <t>DEC_0929</t>
+  </si>
+  <si>
+    <t>DEC_0930</t>
+  </si>
+  <si>
+    <t>DEC_0932</t>
+  </si>
+  <si>
+    <t>DEC_0933</t>
+  </si>
+  <si>
+    <t>DEC_0935</t>
+  </si>
+  <si>
+    <t>DEC_0936</t>
+  </si>
+  <si>
+    <t>DEC_0937</t>
+  </si>
+  <si>
+    <t>DEC_0938</t>
+  </si>
+  <si>
+    <t>DEC_0940</t>
+  </si>
+  <si>
+    <t>DEC_0941</t>
+  </si>
+  <si>
+    <t>DEC_0942</t>
+  </si>
+  <si>
+    <t>DEC_0944</t>
+  </si>
+  <si>
+    <t>DEC_0945</t>
+  </si>
+  <si>
+    <t>DEC_0947</t>
+  </si>
+  <si>
+    <t>DEC_0949</t>
+  </si>
+  <si>
+    <t>DEC_0950</t>
+  </si>
+  <si>
+    <t>DEC_0951</t>
+  </si>
+  <si>
+    <t>DEC_0952</t>
+  </si>
+  <si>
+    <t>DEC_0954</t>
+  </si>
+  <si>
+    <t>DEC_0956</t>
+  </si>
+  <si>
+    <t>DEC_0957</t>
+  </si>
+  <si>
+    <t>DEC_0959</t>
+  </si>
+  <si>
+    <t>DEC_0960</t>
+  </si>
+  <si>
+    <t>DEC_0964</t>
+  </si>
+  <si>
+    <t>DEC_0965</t>
+  </si>
+  <si>
+    <t>DEC_0968</t>
+  </si>
+  <si>
+    <t>DEC_0970</t>
+  </si>
+  <si>
+    <t>DEC_0971</t>
+  </si>
+  <si>
+    <t>DEC_0973</t>
+  </si>
+  <si>
+    <t>DEC_0974</t>
+  </si>
+  <si>
+    <t>DEC_0977</t>
+  </si>
+  <si>
+    <t>DEC_0978</t>
+  </si>
+  <si>
+    <t>DEC_0980</t>
+  </si>
+  <si>
+    <t>DEC_0981</t>
   </si>
 </sst>
 </file>
@@ -693,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O100"/>
+  <dimension ref="A1:O136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="B130" sqref="B130:J130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3273,7 +3387,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>98</v>
       </c>
@@ -3305,7 +3419,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>99</v>
       </c>
@@ -3337,7 +3451,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>100</v>
       </c>
@@ -3369,7 +3483,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>101</v>
       </c>
@@ -3401,7 +3515,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>102</v>
       </c>
@@ -3433,7 +3547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>103</v>
       </c>
@@ -3465,7 +3579,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>104</v>
       </c>
@@ -3497,7 +3611,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>105</v>
       </c>
@@ -3529,7 +3643,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>106</v>
       </c>
@@ -3561,7 +3675,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>107</v>
       </c>
@@ -3593,7 +3707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>108</v>
       </c>
@@ -3625,7 +3739,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>109</v>
       </c>
@@ -3657,86 +3771,1294 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="2"/>
-      <c r="C93" s="3"/>
-    </row>
-    <row r="94" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="2"/>
-      <c r="C94" s="3"/>
-    </row>
-    <row r="95" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="2"/>
-      <c r="C95" s="3"/>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G93" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H93" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I93" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J93" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H94" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I94" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J94" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G95" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H95" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I95" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J95" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J96" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G97" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H97" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I97" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J97" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H98" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I98" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J98" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G99" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H99" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I99" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J99" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G100" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H100" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I100" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J100" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G101" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H101" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I101" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J101" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G102" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H102" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I102" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J102" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G103" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H103" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I103" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J103" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G104" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H104" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I104" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J104" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G105" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H105" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I105" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J105" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G106" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H106" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I106" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J106" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G107" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H107" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I107" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J107" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G108" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H108" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I108" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J108" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F109" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G109" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H109" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I109" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J109" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E110" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F110" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G110" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H110" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I110" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J110" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E111" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G111" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H111" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I111" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J111" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G112" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H112" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I112" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J112" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F113" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G113" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H113" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I113" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J113" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G114" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H114" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I114" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J114" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E115" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F115" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G115" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H115" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I115" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J115" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G116" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H116" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I116" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J116" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F117" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G117" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H117" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I117" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J117" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G118" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H118" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I118" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J118" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E119" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G119" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H119" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I119" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J119" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F120" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G120" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H120" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I120" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J120" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E121" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F121" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G121" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H121" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I121" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J121" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G122" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H122" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I122" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J122" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D123" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E123" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G123" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H123" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I123" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J123" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F124" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G124" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H124" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I124" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J124" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D125" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E125" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F125" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G125" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H125" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I125" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J125" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D126" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E126" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F126" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G126" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H126" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I126" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J126" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D127" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E127" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F127" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G127" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H127" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I127" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J127" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D128" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F128" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G128" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H128" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I128" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J128" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D129" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E129" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F129" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G129" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H129" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I129" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J129" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D130" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E130" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F130" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G130" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H130" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I130" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J130" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B131" s="2"/>
+      <c r="C131" s="3"/>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A132" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B96" s="6" t="s">
+      <c r="B132" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C96" s="6" t="s">
+      <c r="C132" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="D132" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E96" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G96" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H96" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I96" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J96" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K96" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="L96" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M96" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="N96" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="O96" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B97" s="2"/>
-      <c r="C97" s="3"/>
-    </row>
-    <row r="98" spans="2:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="4"/>
-      <c r="C98" s="4"/>
-    </row>
-    <row r="99" spans="2:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="4" t="s">
+      <c r="E132" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F132" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G132" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H132" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I132" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J132" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K132" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L132" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M132" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N132" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O132" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B133" s="2"/>
+      <c r="C133" s="3"/>
+    </row>
+    <row r="134" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B134" s="4"/>
+      <c r="C134" s="4"/>
+    </row>
+    <row r="135" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B135" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C99" s="4" t="s">
+      <c r="C135" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C100" s="3" t="s">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B136" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C136" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test 968 al 1026 MiPortal2
</commit_message>
<xml_diff>
--- a/DataPool.xlsx
+++ b/DataPool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Verity-Usuario\eclipse-workspace\AceptaDec5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348A0FA4-548F-4729-A05F-3F90B8E672ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D55D57-763C-4EAA-8481-92F300FC1DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="165">
   <si>
     <t>18092588-0</t>
   </si>
@@ -478,6 +478,57 @@
   </si>
   <si>
     <t>DEC_0981</t>
+  </si>
+  <si>
+    <t>DEC_0984</t>
+  </si>
+  <si>
+    <t>DEC_0985</t>
+  </si>
+  <si>
+    <t>DEC_0986</t>
+  </si>
+  <si>
+    <t>DEC_0988</t>
+  </si>
+  <si>
+    <t>DEC_0989</t>
+  </si>
+  <si>
+    <t>DEC_0990</t>
+  </si>
+  <si>
+    <t>DEC_0993</t>
+  </si>
+  <si>
+    <t>DEC_0997</t>
+  </si>
+  <si>
+    <t>DEC_0998</t>
+  </si>
+  <si>
+    <t>DEC_0999</t>
+  </si>
+  <si>
+    <t>DEC_1000</t>
+  </si>
+  <si>
+    <t>DEC_1002</t>
+  </si>
+  <si>
+    <t>DEC_1003</t>
+  </si>
+  <si>
+    <t>DEC_1004</t>
+  </si>
+  <si>
+    <t>DEC_1005</t>
+  </si>
+  <si>
+    <t>DEC_1025</t>
+  </si>
+  <si>
+    <t>DEC_1026</t>
   </si>
 </sst>
 </file>
@@ -807,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O136"/>
+  <dimension ref="A1:O158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="B130" sqref="B130:J130"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="C150" sqref="C150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4923,7 +4974,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="129" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>146</v>
       </c>
@@ -4955,7 +5006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="130" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>147</v>
       </c>
@@ -4987,78 +5038,642 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B131" s="2"/>
-      <c r="C131" s="3"/>
-    </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D131" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E131" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F131" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G131" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H131" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I131" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J131" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D132" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E132" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F132" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G132" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H132" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I132" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J132" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D133" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E133" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F133" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G133" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H133" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I133" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J133" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D134" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E134" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F134" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G134" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H134" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I134" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J134" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D135" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E135" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F135" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G135" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H135" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I135" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J135" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E136" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F136" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G136" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H136" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I136" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J136" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D137" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E137" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F137" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G137" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H137" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I137" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J137" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D138" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E138" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F138" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G138" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H138" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I138" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J138" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D139" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E139" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F139" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G139" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H139" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I139" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J139" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D140" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E140" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F140" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G140" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H140" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I140" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J140" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D141" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E141" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F141" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G141" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H141" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I141" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J141" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D142" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E142" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F142" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G142" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H142" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I142" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J142" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D143" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E143" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F143" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G143" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H143" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I143" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J143" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D144" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E144" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F144" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G144" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H144" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I144" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J144" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D145" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E145" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F145" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G145" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H145" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I145" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J145" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D146" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E146" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F146" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G146" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H146" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I146" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J146" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D147" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E147" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F147" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G147" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H147" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I147" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J147" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B148" s="2"/>
+      <c r="C148" s="3"/>
+    </row>
+    <row r="149" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B149" s="2"/>
+      <c r="C149" s="3"/>
+    </row>
+    <row r="150" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B150" s="2"/>
+      <c r="C150" s="3"/>
+    </row>
+    <row r="151" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B151" s="2"/>
+      <c r="C151" s="3"/>
+    </row>
+    <row r="152" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B152" s="2"/>
+      <c r="C152" s="3"/>
+    </row>
+    <row r="153" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B153" s="2"/>
+      <c r="C153" s="3"/>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A154" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B132" s="6" t="s">
+      <c r="B154" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C132" s="6" t="s">
+      <c r="C154" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D132" s="5" t="s">
+      <c r="D154" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E132" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F132" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G132" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H132" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I132" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J132" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K132" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="L132" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M132" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="N132" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="O132" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B133" s="2"/>
-      <c r="C133" s="3"/>
-    </row>
-    <row r="134" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B134" s="4"/>
-      <c r="C134" s="4"/>
-    </row>
-    <row r="135" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="4" t="s">
+      <c r="E154" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F154" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G154" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H154" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I154" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J154" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K154" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L154" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M154" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N154" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O154" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B155" s="2"/>
+      <c r="C155" s="3"/>
+    </row>
+    <row r="156" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B156" s="4"/>
+      <c r="C156" s="4"/>
+    </row>
+    <row r="157" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B157" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C135" s="4" t="s">
+      <c r="C157" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B136" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C136" s="3" t="s">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B158" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C158" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>